<commit_message>
append new init data
</commit_message>
<xml_diff>
--- a/core-db/src/main/java/hap/extend/core/db/data/2017-03-22-init-data.xlsx
+++ b/core-db/src/main/java/hap/extend/core/db/data/2017-03-22-init-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="566" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="566" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1267,10 +1267,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>hap_extend.op_permission.grid_title.componentType</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>具体类型</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -1279,15 +1275,7 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>hap_extend.op_permission.grid_title.htmlTagAttr</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>HTML标签属性</t>
-  </si>
-  <si>
-    <t>hap_extend.op_permission.grid_title.htmlTagAttrVal</t>
-    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HTML标签属性值</t>
@@ -1841,6 +1829,18 @@
   </si>
   <si>
     <t>fetch menu structure</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>hap_extend.op_permission.grid_title.component_type</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>hap_extend.op_permission.grid_title.html_tag_attr</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>hap_extend.op_permission.grid_title.html_tag_attr_val</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -2096,8 +2096,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2274,7 +2276,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
@@ -2299,6 +2301,7 @@
     <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -2322,6 +2325,7 @@
     <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -3353,7 +3357,7 @@
   <sheetPr codeName="工作表3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:B45"/>
     </sheetView>
   </sheetViews>
@@ -3481,7 +3485,7 @@
         <v>199</v>
       </c>
       <c r="F8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G8" t="s">
         <v>92</v>
@@ -3933,10 +3937,10 @@
         <v>192</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F21" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G21" t="s">
         <v>92</v>
@@ -3948,16 +3952,16 @@
         <v>179</v>
       </c>
       <c r="J21" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K21" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L21" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="M21" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -3968,10 +3972,10 @@
         <v>192</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F22" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G22" t="s">
         <v>92</v>
@@ -3983,16 +3987,16 @@
         <v>195</v>
       </c>
       <c r="J22" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K22" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="L22" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="M22" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4003,10 +4007,10 @@
         <v>192</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F23" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G23" t="s">
         <v>92</v>
@@ -4018,16 +4022,16 @@
         <v>179</v>
       </c>
       <c r="J23" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="K23" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L23" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="M23" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -4038,10 +4042,10 @@
         <v>192</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F24" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G24" t="s">
         <v>92</v>
@@ -4053,16 +4057,16 @@
         <v>195</v>
       </c>
       <c r="J24" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K24" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="L24" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="M24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -4073,10 +4077,10 @@
         <v>192</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F25" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G25" t="s">
         <v>92</v>
@@ -4088,16 +4092,16 @@
         <v>179</v>
       </c>
       <c r="J25" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="K25" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="L25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M25" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -4108,10 +4112,10 @@
         <v>192</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F26" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
@@ -4123,16 +4127,16 @@
         <v>195</v>
       </c>
       <c r="J26" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="K26" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="L26" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="M26" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -4143,10 +4147,10 @@
         <v>192</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F27" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G27" t="s">
         <v>92</v>
@@ -4158,16 +4162,16 @@
         <v>179</v>
       </c>
       <c r="J27" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="K27" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="L27" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="M27" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4178,10 +4182,10 @@
         <v>192</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F28" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G28" t="s">
         <v>94</v>
@@ -4193,16 +4197,16 @@
         <v>93</v>
       </c>
       <c r="J28" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="K28" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="L28" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="M28" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -4213,10 +4217,10 @@
         <v>192</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F29" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G29" t="s">
         <v>94</v>
@@ -4228,16 +4232,16 @@
         <v>93</v>
       </c>
       <c r="J29" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="K29" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="L29" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="M29" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -4248,10 +4252,10 @@
         <v>192</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G30" t="s">
         <v>94</v>
@@ -4263,16 +4267,16 @@
         <v>93</v>
       </c>
       <c r="J30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="K30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="L30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="M30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -4283,10 +4287,10 @@
         <v>192</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F31" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G31" t="s">
         <v>94</v>
@@ -4298,16 +4302,16 @@
         <v>93</v>
       </c>
       <c r="J31" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="K31" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="L31" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="M31" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4318,10 +4322,10 @@
         <v>192</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F32" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G32" t="s">
         <v>94</v>
@@ -4333,16 +4337,16 @@
         <v>93</v>
       </c>
       <c r="J32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="K32" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="L32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="M32" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4353,10 +4357,10 @@
         <v>192</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F33" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G33" t="s">
         <v>94</v>
@@ -4368,16 +4372,16 @@
         <v>93</v>
       </c>
       <c r="J33" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="K33" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="L33" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="M33" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4388,10 +4392,10 @@
         <v>192</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F34" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G34" t="s">
         <v>94</v>
@@ -4403,16 +4407,16 @@
         <v>93</v>
       </c>
       <c r="J34" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="K34" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="L34" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="M34" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -4423,10 +4427,10 @@
         <v>192</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F35" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G35" t="s">
         <v>94</v>
@@ -4438,16 +4442,16 @@
         <v>93</v>
       </c>
       <c r="J35" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="K35" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="L35" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="M35" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -4458,10 +4462,10 @@
         <v>192</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F36" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G36" t="s">
         <v>94</v>
@@ -4473,16 +4477,16 @@
         <v>93</v>
       </c>
       <c r="J36" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="K36" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="L36" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="M36" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -4493,10 +4497,10 @@
         <v>192</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F37" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G37" t="s">
         <v>94</v>
@@ -4508,16 +4512,16 @@
         <v>93</v>
       </c>
       <c r="J37" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="K37" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="L37" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="M37" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -4528,10 +4532,10 @@
         <v>192</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F38" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G38" t="s">
         <v>94</v>
@@ -4543,16 +4547,16 @@
         <v>93</v>
       </c>
       <c r="J38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K38" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="L38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M38" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -4563,10 +4567,10 @@
         <v>192</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F39" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G39" t="s">
         <v>94</v>
@@ -4578,16 +4582,16 @@
         <v>93</v>
       </c>
       <c r="J39" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="K39" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="L39" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M39" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -4598,10 +4602,10 @@
         <v>192</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F40" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G40" t="s">
         <v>94</v>
@@ -4613,16 +4617,16 @@
         <v>93</v>
       </c>
       <c r="J40" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="K40" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="L40" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M40" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -4633,10 +4637,10 @@
         <v>192</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F41" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G41" t="s">
         <v>94</v>
@@ -4648,16 +4652,16 @@
         <v>93</v>
       </c>
       <c r="J41" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="K41" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="L41" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="M41" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -4668,10 +4672,10 @@
         <v>192</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F42" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G42" t="s">
         <v>94</v>
@@ -4683,16 +4687,16 @@
         <v>93</v>
       </c>
       <c r="J42" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K42" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L42" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="M42" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -4703,10 +4707,10 @@
         <v>192</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F43" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G43" t="s">
         <v>94</v>
@@ -4718,16 +4722,16 @@
         <v>93</v>
       </c>
       <c r="J43" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="K43" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="L43" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="M43" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -4738,10 +4742,10 @@
         <v>192</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F44" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G44" t="s">
         <v>94</v>
@@ -4753,16 +4757,16 @@
         <v>93</v>
       </c>
       <c r="J44" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="K44" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="L44" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="M44" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -4773,10 +4777,10 @@
         <v>192</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F45" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G45" t="s">
         <v>94</v>
@@ -4788,16 +4792,16 @@
         <v>93</v>
       </c>
       <c r="J45" t="s">
+        <v>415</v>
+      </c>
+      <c r="K45" t="s">
         <v>418</v>
       </c>
-      <c r="K45" t="s">
-        <v>421</v>
-      </c>
       <c r="L45" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="M45" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -5194,7 +5198,7 @@
     </row>
     <row r="25" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E25" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F25" s="16" t="str">
         <f>$E$9</f>
@@ -5207,7 +5211,7 @@
     </row>
     <row r="26" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E26" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F26" s="16" t="str">
         <f>$E$9</f>
@@ -5220,10 +5224,10 @@
     </row>
     <row r="27" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E27" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F27" s="16" t="str">
-        <f t="shared" ref="F27:F35" si="0">$E$9</f>
+        <f t="shared" ref="F27:F32" si="0">$E$9</f>
         <v>HAP_EXTEND_OPT_PERMISSION</v>
       </c>
       <c r="G27" s="16" t="str">
@@ -5233,7 +5237,7 @@
     </row>
     <row r="28" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E28" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F28" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5246,7 +5250,7 @@
     </row>
     <row r="29" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E29" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F29" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5259,7 +5263,7 @@
     </row>
     <row r="30" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E30" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F30" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5272,7 +5276,7 @@
     </row>
     <row r="31" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E31" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F31" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5285,7 +5289,7 @@
     </row>
     <row r="32" spans="4:22" x14ac:dyDescent="0.2">
       <c r="E32" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F32" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5623,8 +5627,8 @@
   <sheetPr codeName="工作表6" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H341"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6089,7 +6093,7 @@
         <v>80</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>123</v>
@@ -6117,13 +6121,13 @@
         <v>80</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>289</v>
+        <v>419</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.2">
@@ -6131,13 +6135,13 @@
         <v>80</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>289</v>
+        <v>419</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.2">
@@ -6145,13 +6149,13 @@
         <v>80</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>292</v>
+        <v>420</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.2">
@@ -6159,13 +6163,13 @@
         <v>80</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>292</v>
+        <v>420</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42" spans="5:8" x14ac:dyDescent="0.2">
@@ -6173,13 +6177,13 @@
         <v>80</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>294</v>
+        <v>421</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="5:8" x14ac:dyDescent="0.2">
@@ -6187,13 +6191,13 @@
         <v>80</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>294</v>
+        <v>421</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="5:8" x14ac:dyDescent="0.2">
@@ -6201,13 +6205,13 @@
         <v>80</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="5:8" x14ac:dyDescent="0.2">
@@ -6215,13 +6219,13 @@
         <v>80</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="5:8" x14ac:dyDescent="0.2">
@@ -6229,13 +6233,13 @@
         <v>80</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="5:8" x14ac:dyDescent="0.2">
@@ -6243,13 +6247,13 @@
         <v>80</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" spans="5:8" x14ac:dyDescent="0.2">
@@ -6257,13 +6261,13 @@
         <v>80</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.2">
@@ -6271,13 +6275,13 @@
         <v>80</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.2">
@@ -6285,13 +6289,13 @@
         <v>80</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="51" spans="5:8" x14ac:dyDescent="0.2">
@@ -6299,13 +6303,13 @@
         <v>80</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.2">
@@ -6313,13 +6317,13 @@
         <v>80</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.2">
@@ -6327,13 +6331,13 @@
         <v>80</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.2">
@@ -6341,13 +6345,13 @@
         <v>80</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="5:8" x14ac:dyDescent="0.2">
@@ -6355,13 +6359,13 @@
         <v>80</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.2">
@@ -6369,13 +6373,13 @@
         <v>80</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.2">
@@ -6383,13 +6387,13 @@
         <v>80</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="5:8" x14ac:dyDescent="0.2">
@@ -6397,13 +6401,13 @@
         <v>80</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.2">
@@ -6411,13 +6415,13 @@
         <v>80</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="5:8" x14ac:dyDescent="0.2">
@@ -6425,13 +6429,13 @@
         <v>80</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>123</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="5:8" x14ac:dyDescent="0.2">
@@ -6439,13 +6443,13 @@
         <v>80</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>124</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="5:8" x14ac:dyDescent="0.2">

</xml_diff>